<commit_message>
add a new mean reversion strat: one based on GARCH(1,1) model
</commit_message>
<xml_diff>
--- a/results/compTable.xlsx
+++ b/results/compTable.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,11 @@
           <t>third</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>GARCH</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -465,6 +470,9 @@
       <c r="D2" t="n">
         <v>0.8100000000000001</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.43</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -481,6 +489,9 @@
       <c r="D3" t="n">
         <v>1.34</v>
       </c>
+      <c r="E3" t="n">
+        <v>0.65</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -497,6 +508,9 @@
       <c r="D4" t="n">
         <v>0.01</v>
       </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -513,6 +527,9 @@
       <c r="D5" t="n">
         <v>16310.18</v>
       </c>
+      <c r="E5" t="n">
+        <v>1219584.15</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -529,6 +546,9 @@
       <c r="D6" t="n">
         <v>13087.48</v>
       </c>
+      <c r="E6" t="n">
+        <v>2408660.67</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -545,6 +565,9 @@
       <c r="D7" t="n">
         <v>0.8024</v>
       </c>
+      <c r="E7" t="n">
+        <v>1.975</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -561,6 +584,9 @@
       <c r="D8" t="n">
         <v>0.2641</v>
       </c>
+      <c r="E8" t="n">
+        <v>0.1821</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -577,6 +603,9 @@
       <c r="D9" t="n">
         <v>0.0862</v>
       </c>
+      <c r="E9" t="n">
+        <v>0.2944</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -593,6 +622,9 @@
       <c r="D10" t="n">
         <v>1.35</v>
       </c>
+      <c r="E10" t="n">
+        <v>1.77</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -609,6 +641,9 @@
       <c r="D11" t="n">
         <v>3</v>
       </c>
+      <c r="E11" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -625,6 +660,9 @@
       <c r="D12" t="n">
         <v>3028</v>
       </c>
+      <c r="E12" t="n">
+        <v>4549</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -641,6 +679,9 @@
       <c r="D13" t="n">
         <v>0.001</v>
       </c>
+      <c r="E13" t="n">
+        <v>0.0004</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -657,6 +698,9 @@
       <c r="D14" t="n">
         <v>0.678996036988111</v>
       </c>
+      <c r="E14" t="n">
+        <v>0.7610343290236291</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
@@ -673,6 +717,9 @@
       <c r="D15" t="n">
         <v>0.01417253168727139</v>
       </c>
+      <c r="E15" t="n">
+        <v>0.1489108761279314</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
@@ -689,6 +736,9 @@
       <c r="D16" t="n">
         <v>-0.0182724780043938</v>
       </c>
+      <c r="E16" t="n">
+        <v>-0.06610456994113106</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
@@ -704,6 +754,9 @@
       </c>
       <c r="D17" t="n">
         <v>0.004769915331074102</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.1122050666664724</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add a new strategy: mean reversion with a avg rolling vol model
</commit_message>
<xml_diff>
--- a/results/compTable.xlsx
+++ b/results/compTable.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,6 +451,11 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>SimpleVol</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>GARCH</t>
         </is>
       </c>
@@ -471,6 +476,9 @@
         <v>0.8100000000000001</v>
       </c>
       <c r="E2" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="F2" t="n">
         <v>0.43</v>
       </c>
     </row>
@@ -490,6 +498,9 @@
         <v>1.34</v>
       </c>
       <c r="E3" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="F3" t="n">
         <v>0.65</v>
       </c>
     </row>
@@ -511,6 +522,9 @@
       <c r="E4" t="n">
         <v>0</v>
       </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -528,6 +542,9 @@
         <v>16310.18</v>
       </c>
       <c r="E5" t="n">
+        <v>879163.61</v>
+      </c>
+      <c r="F5" t="n">
         <v>1219584.15</v>
       </c>
     </row>
@@ -547,6 +564,9 @@
         <v>13087.48</v>
       </c>
       <c r="E6" t="n">
+        <v>1805830.02</v>
+      </c>
+      <c r="F6" t="n">
         <v>2408660.67</v>
       </c>
     </row>
@@ -566,6 +586,9 @@
         <v>0.8024</v>
       </c>
       <c r="E7" t="n">
+        <v>2.054</v>
+      </c>
+      <c r="F7" t="n">
         <v>1.975</v>
       </c>
     </row>
@@ -585,6 +608,9 @@
         <v>0.2641</v>
       </c>
       <c r="E8" t="n">
+        <v>0.1907</v>
+      </c>
+      <c r="F8" t="n">
         <v>0.1821</v>
       </c>
     </row>
@@ -604,6 +630,9 @@
         <v>0.0862</v>
       </c>
       <c r="E9" t="n">
+        <v>0.2976</v>
+      </c>
+      <c r="F9" t="n">
         <v>0.2944</v>
       </c>
     </row>
@@ -623,6 +652,9 @@
         <v>1.35</v>
       </c>
       <c r="E10" t="n">
+        <v>1.78</v>
+      </c>
+      <c r="F10" t="n">
         <v>1.77</v>
       </c>
     </row>
@@ -644,6 +676,9 @@
       <c r="E11" t="n">
         <v>3</v>
       </c>
+      <c r="F11" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -661,6 +696,9 @@
         <v>3028</v>
       </c>
       <c r="E12" t="n">
+        <v>4703</v>
+      </c>
+      <c r="F12" t="n">
         <v>4549</v>
       </c>
     </row>
@@ -682,6 +720,9 @@
       <c r="E13" t="n">
         <v>0.0004</v>
       </c>
+      <c r="F13" t="n">
+        <v>0.0004</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -699,6 +740,9 @@
         <v>0.678996036988111</v>
       </c>
       <c r="E14" t="n">
+        <v>0.7502134927412468</v>
+      </c>
+      <c r="F14" t="n">
         <v>0.7610343290236291</v>
       </c>
     </row>
@@ -718,6 +762,9 @@
         <v>0.01417253168727139</v>
       </c>
       <c r="E15" t="n">
+        <v>0.1185323742343591</v>
+      </c>
+      <c r="F15" t="n">
         <v>0.1489108761279314</v>
       </c>
     </row>
@@ -737,6 +784,9 @@
         <v>-0.0182724780043938</v>
       </c>
       <c r="E16" t="n">
+        <v>-0.04126801097872668</v>
+      </c>
+      <c r="F16" t="n">
         <v>-0.06610456994113106</v>
       </c>
     </row>
@@ -756,6 +806,9 @@
         <v>0.004769915331074102</v>
       </c>
       <c r="E17" t="n">
+        <v>0.08972962485051468</v>
+      </c>
+      <c r="F17" t="n">
         <v>0.1122050666664724</v>
       </c>
     </row>

</xml_diff>